<commit_message>
updated risk_id's so there are more than just AP
</commit_message>
<xml_diff>
--- a/clensed.xlsx
+++ b/clensed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PythonProjects\wip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3824E424-6733-461D-A9E7-0B80493450DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BE532A-A47D-408C-AF36-621393BAE501}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7757194A-FA31-4D25-A9B8-7AE7E2677B79}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7757194A-FA31-4D25-A9B8-7AE7E2677B79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1303,150 +1303,6 @@
     <t>AP-P01-R04</t>
   </si>
   <si>
-    <t>AP-P02-R05</t>
-  </si>
-  <si>
-    <t>AP-P03-R06</t>
-  </si>
-  <si>
-    <t>AP-P01-R07</t>
-  </si>
-  <si>
-    <t>AP-P02-R08</t>
-  </si>
-  <si>
-    <t>AP-P03-R09</t>
-  </si>
-  <si>
-    <t>AP-P01-R10</t>
-  </si>
-  <si>
-    <t>AP-P02-R11</t>
-  </si>
-  <si>
-    <t>AP-P03-R12</t>
-  </si>
-  <si>
-    <t>AP-P01-R13</t>
-  </si>
-  <si>
-    <t>AP-P02-R14</t>
-  </si>
-  <si>
-    <t>AP-P03-R15</t>
-  </si>
-  <si>
-    <t>AP-P01-R16</t>
-  </si>
-  <si>
-    <t>AP-P02-R17</t>
-  </si>
-  <si>
-    <t>AP-P03-R18</t>
-  </si>
-  <si>
-    <t>AP-P01-R19</t>
-  </si>
-  <si>
-    <t>AP-P02-R20</t>
-  </si>
-  <si>
-    <t>AP-P03-R21</t>
-  </si>
-  <si>
-    <t>AP-P01-R22</t>
-  </si>
-  <si>
-    <t>AP-P02-R23</t>
-  </si>
-  <si>
-    <t>AP-P03-R24</t>
-  </si>
-  <si>
-    <t>AP-P01-R25</t>
-  </si>
-  <si>
-    <t>AP-P02-R26</t>
-  </si>
-  <si>
-    <t>AP-P03-R27</t>
-  </si>
-  <si>
-    <t>AP-P01-R28</t>
-  </si>
-  <si>
-    <t>AP-P02-R29</t>
-  </si>
-  <si>
-    <t>AP-P03-R30</t>
-  </si>
-  <si>
-    <t>AP-P01-R31</t>
-  </si>
-  <si>
-    <t>AP-P02-R32</t>
-  </si>
-  <si>
-    <t>AP-P03-R33</t>
-  </si>
-  <si>
-    <t>AP-P01-R34</t>
-  </si>
-  <si>
-    <t>AP-P02-R35</t>
-  </si>
-  <si>
-    <t>AP-P03-R36</t>
-  </si>
-  <si>
-    <t>AP-P01-R37</t>
-  </si>
-  <si>
-    <t>AP-P02-R38</t>
-  </si>
-  <si>
-    <t>AP-P03-R39</t>
-  </si>
-  <si>
-    <t>AP-P01-R40</t>
-  </si>
-  <si>
-    <t>AP-P02-R41</t>
-  </si>
-  <si>
-    <t>AP-P03-R42</t>
-  </si>
-  <si>
-    <t>AP-P01-R42</t>
-  </si>
-  <si>
-    <t>AP-P02-R44</t>
-  </si>
-  <si>
-    <t>AP-P03-R45</t>
-  </si>
-  <si>
-    <t>AP-P01-R46</t>
-  </si>
-  <si>
-    <t>AP-P02-R47</t>
-  </si>
-  <si>
-    <t>AP-P03-R48</t>
-  </si>
-  <si>
-    <t>AP-P01-R49</t>
-  </si>
-  <si>
-    <t>AP-P02-R50</t>
-  </si>
-  <si>
-    <t>AP-P03-R51</t>
-  </si>
-  <si>
-    <t>AP-P01-R52</t>
-  </si>
-  <si>
     <t>Description 1</t>
   </si>
   <si>
@@ -2142,6 +1998,150 @@
   </si>
   <si>
     <t>Regulatory &amp; Compliance Risk</t>
+  </si>
+  <si>
+    <t>BP-P01-R01</t>
+  </si>
+  <si>
+    <t>BP-P01-R02</t>
+  </si>
+  <si>
+    <t>BP-P01-R03</t>
+  </si>
+  <si>
+    <t>BP-P01-R04</t>
+  </si>
+  <si>
+    <t>BP-P01-R05</t>
+  </si>
+  <si>
+    <t>BP-P01-R06</t>
+  </si>
+  <si>
+    <t>BP-P01-R07</t>
+  </si>
+  <si>
+    <t>CP-P01-R01</t>
+  </si>
+  <si>
+    <t>CP-P01-R02</t>
+  </si>
+  <si>
+    <t>CP-P01-R03</t>
+  </si>
+  <si>
+    <t>CP-P01-R04</t>
+  </si>
+  <si>
+    <t>CP-P01-R05</t>
+  </si>
+  <si>
+    <t>CP-P01-R06</t>
+  </si>
+  <si>
+    <t>CP-P01-R07</t>
+  </si>
+  <si>
+    <t>CP-P01-R08</t>
+  </si>
+  <si>
+    <t>DP-P01-R01</t>
+  </si>
+  <si>
+    <t>DP-P01-R02</t>
+  </si>
+  <si>
+    <t>DP-P01-R03</t>
+  </si>
+  <si>
+    <t>DP-P01-R04</t>
+  </si>
+  <si>
+    <t>DP-P01-R05</t>
+  </si>
+  <si>
+    <t>DP-P01-R06</t>
+  </si>
+  <si>
+    <t>DP-P01-R07</t>
+  </si>
+  <si>
+    <t>DP-P01-R08</t>
+  </si>
+  <si>
+    <t>DP-P01-R09</t>
+  </si>
+  <si>
+    <t>DP-P01-R10</t>
+  </si>
+  <si>
+    <t>DP-P01-R11</t>
+  </si>
+  <si>
+    <t>DP-P01-R12</t>
+  </si>
+  <si>
+    <t>DP-P01-R13</t>
+  </si>
+  <si>
+    <t>DP-P01-R14</t>
+  </si>
+  <si>
+    <t>DP-P01-R15</t>
+  </si>
+  <si>
+    <t>DP-P01-R16</t>
+  </si>
+  <si>
+    <t>DP-P01-R17</t>
+  </si>
+  <si>
+    <t>DP-P01-R18</t>
+  </si>
+  <si>
+    <t>DP-P01-R19</t>
+  </si>
+  <si>
+    <t>DP-P01-R20</t>
+  </si>
+  <si>
+    <t>DP-P01-R21</t>
+  </si>
+  <si>
+    <t>DP-P01-R22</t>
+  </si>
+  <si>
+    <t>DP-P01-R23</t>
+  </si>
+  <si>
+    <t>DP-P01-R24</t>
+  </si>
+  <si>
+    <t>DP-P01-R25</t>
+  </si>
+  <si>
+    <t>DP-P01-R26</t>
+  </si>
+  <si>
+    <t>DP-P01-R27</t>
+  </si>
+  <si>
+    <t>DP-P01-R28</t>
+  </si>
+  <si>
+    <t>DP-P01-R29</t>
+  </si>
+  <si>
+    <t>DP-P01-R30</t>
+  </si>
+  <si>
+    <t>DP-P01-R31</t>
+  </si>
+  <si>
+    <t>DP-P01-R32</t>
+  </si>
+  <si>
+    <t>DP-P01-R33</t>
   </si>
 </sst>
 </file>
@@ -3313,11 +3313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35F8A17-9F7B-467B-9749-779D87641394}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AI391"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3452,24 +3451,24 @@
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
     </row>
-    <row r="2" spans="1:35" ht="140.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>166</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>322</v>
+        <v>274</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>270</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>476</v>
+        <v>428</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>218</v>
       </c>
       <c r="F2" s="69" t="s">
-        <v>374</v>
+        <v>326</v>
       </c>
       <c r="G2" s="65" t="s">
         <v>28</v>
@@ -3490,16 +3489,16 @@
         <v>3</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>486</v>
+        <v>438</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>476</v>
+        <v>428</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>30</v>
       </c>
       <c r="P2" s="70" t="s">
-        <v>426</v>
+        <v>378</v>
       </c>
       <c r="Q2" s="24" t="s">
         <v>31</v>
@@ -3539,24 +3538,24 @@
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="1:35" ht="223.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="223.5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>167</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>323</v>
+        <v>275</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>271</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>476</v>
+        <v>428</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>219</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>375</v>
+        <v>327</v>
       </c>
       <c r="G3" s="65" t="s">
         <v>28</v>
@@ -3577,16 +3576,16 @@
         <v>3</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>485</v>
+        <v>437</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>476</v>
+        <v>428</v>
       </c>
       <c r="O3" s="24" t="s">
         <v>38</v>
       </c>
       <c r="P3" s="71" t="s">
-        <v>427</v>
+        <v>379</v>
       </c>
       <c r="Q3" s="24" t="s">
         <v>31</v>
@@ -3626,24 +3625,24 @@
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
     </row>
-    <row r="4" spans="1:35" ht="223.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="223.5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>168</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>324</v>
+        <v>276</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>272</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>476</v>
+        <v>428</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>220</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>376</v>
+        <v>328</v>
       </c>
       <c r="G4" s="65" t="s">
         <v>28</v>
@@ -3664,16 +3663,16 @@
         <v>3</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>487</v>
+        <v>439</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>476</v>
+        <v>428</v>
       </c>
       <c r="O4" s="24" t="s">
         <v>41</v>
       </c>
       <c r="P4" s="71" t="s">
-        <v>428</v>
+        <v>380</v>
       </c>
       <c r="Q4" s="24" t="s">
         <v>31</v>
@@ -3713,24 +3712,24 @@
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
     </row>
-    <row r="5" spans="1:35" ht="209.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="209.25" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>273</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>476</v>
+        <v>428</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>221</v>
       </c>
       <c r="F5" s="69" t="s">
-        <v>377</v>
+        <v>329</v>
       </c>
       <c r="G5" s="65" t="s">
         <v>28</v>
@@ -3751,16 +3750,16 @@
         <v>3</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>488</v>
+        <v>440</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>476</v>
+        <v>428</v>
       </c>
       <c r="O5" s="24" t="s">
         <v>43</v>
       </c>
       <c r="P5" s="71" t="s">
-        <v>429</v>
+        <v>381</v>
       </c>
       <c r="Q5" s="24" t="s">
         <v>31</v>
@@ -3800,24 +3799,24 @@
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
     </row>
-    <row r="6" spans="1:35" ht="180.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>170</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>326</v>
+        <v>278</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>274</v>
+        <v>490</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>222</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>378</v>
+        <v>330</v>
       </c>
       <c r="G6" s="65" t="s">
         <v>28</v>
@@ -3838,16 +3837,16 @@
         <v>3</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>489</v>
+        <v>441</v>
       </c>
       <c r="N6" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O6" s="24" t="s">
         <v>43</v>
       </c>
       <c r="P6" s="71" t="s">
-        <v>430</v>
+        <v>382</v>
       </c>
       <c r="Q6" s="24" t="s">
         <v>31</v>
@@ -3887,24 +3886,24 @@
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
     </row>
-    <row r="7" spans="1:35" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" ht="116.25" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>171</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>327</v>
+        <v>279</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>275</v>
+        <v>491</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>223</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>379</v>
+        <v>331</v>
       </c>
       <c r="G7" s="65" t="s">
         <v>28</v>
@@ -3925,16 +3924,16 @@
         <v>3</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>490</v>
+        <v>442</v>
       </c>
       <c r="N7" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O7" s="24" t="s">
         <v>47</v>
       </c>
       <c r="P7" s="71" t="s">
-        <v>431</v>
+        <v>383</v>
       </c>
       <c r="Q7" s="24" t="s">
         <v>31</v>
@@ -3974,24 +3973,24 @@
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
     </row>
-    <row r="8" spans="1:35" ht="132.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="136.5" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>172</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>276</v>
+        <v>492</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>224</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>380</v>
+        <v>332</v>
       </c>
       <c r="G8" s="65" t="s">
         <v>28</v>
@@ -4012,16 +4011,16 @@
         <v>3</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>491</v>
+        <v>443</v>
       </c>
       <c r="N8" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O8" s="24" t="s">
         <v>49</v>
       </c>
       <c r="P8" s="71" t="s">
-        <v>432</v>
+        <v>384</v>
       </c>
       <c r="Q8" s="24" t="s">
         <v>31</v>
@@ -4061,24 +4060,24 @@
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
     </row>
-    <row r="9" spans="1:35" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="116.25" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>173</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>277</v>
+        <v>493</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>225</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>381</v>
+        <v>333</v>
       </c>
       <c r="G9" s="66" t="s">
         <v>28</v>
@@ -4099,16 +4098,16 @@
         <v>5</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>492</v>
+        <v>444</v>
       </c>
       <c r="N9" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O9" s="24" t="s">
         <v>53</v>
       </c>
       <c r="P9" s="71" t="s">
-        <v>433</v>
+        <v>385</v>
       </c>
       <c r="Q9" s="24" t="s">
         <v>31</v>
@@ -4148,24 +4147,24 @@
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
     </row>
-    <row r="10" spans="1:35" ht="145.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="149.25" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>174</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>330</v>
+        <v>282</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>278</v>
+        <v>494</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>226</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>382</v>
+        <v>334</v>
       </c>
       <c r="G10" s="66" t="s">
         <v>28</v>
@@ -4186,16 +4185,16 @@
         <v>5</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>493</v>
+        <v>445</v>
       </c>
       <c r="N10" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O10" s="24" t="s">
         <v>56</v>
       </c>
       <c r="P10" s="71" t="s">
-        <v>434</v>
+        <v>386</v>
       </c>
       <c r="Q10" s="24" t="s">
         <v>31</v>
@@ -4235,24 +4234,24 @@
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
     </row>
-    <row r="11" spans="1:35" ht="156" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="160.5" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>175</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>331</v>
+        <v>283</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>279</v>
+        <v>495</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>227</v>
       </c>
       <c r="F11" s="69" t="s">
-        <v>383</v>
+        <v>335</v>
       </c>
       <c r="G11" s="66" t="s">
         <v>57</v>
@@ -4273,16 +4272,16 @@
         <v>5</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>494</v>
+        <v>446</v>
       </c>
       <c r="N11" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O11" s="24" t="s">
         <v>59</v>
       </c>
       <c r="P11" s="71" t="s">
-        <v>435</v>
+        <v>387</v>
       </c>
       <c r="Q11" s="24" t="s">
         <v>31</v>
@@ -4322,24 +4321,24 @@
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
     </row>
-    <row r="12" spans="1:35" ht="156" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="160.5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>176</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>332</v>
+        <v>284</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>280</v>
+        <v>496</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>228</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>384</v>
+        <v>336</v>
       </c>
       <c r="G12" s="66" t="s">
         <v>28</v>
@@ -4360,16 +4359,16 @@
         <v>2</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>495</v>
+        <v>447</v>
       </c>
       <c r="N12" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O12" s="24" t="s">
         <v>61</v>
       </c>
       <c r="P12" s="71" t="s">
-        <v>436</v>
+        <v>388</v>
       </c>
       <c r="Q12" s="24" t="s">
         <v>62</v>
@@ -4409,24 +4408,24 @@
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
     </row>
-    <row r="13" spans="1:35" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="168.75" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>177</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>333</v>
+        <v>285</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>281</v>
+        <v>497</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>229</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>385</v>
+        <v>337</v>
       </c>
       <c r="G13" s="66" t="s">
         <v>28</v>
@@ -4447,16 +4446,16 @@
         <v>3</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>496</v>
+        <v>448</v>
       </c>
       <c r="N13" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O13" s="24" t="s">
         <v>63</v>
       </c>
       <c r="P13" s="71" t="s">
-        <v>437</v>
+        <v>389</v>
       </c>
       <c r="Q13" s="24" t="s">
         <v>62</v>
@@ -4496,24 +4495,24 @@
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
     </row>
-    <row r="14" spans="1:35" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="168.75" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>178</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>334</v>
+        <v>286</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>282</v>
+        <v>498</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>230</v>
       </c>
       <c r="F14" s="69" t="s">
-        <v>386</v>
+        <v>338</v>
       </c>
       <c r="G14" s="66" t="s">
         <v>28</v>
@@ -4534,16 +4533,16 @@
         <v>3</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>497</v>
+        <v>449</v>
       </c>
       <c r="N14" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O14" s="24" t="s">
         <v>64</v>
       </c>
       <c r="P14" s="71" t="s">
-        <v>438</v>
+        <v>390</v>
       </c>
       <c r="Q14" s="24" t="s">
         <v>62</v>
@@ -4583,24 +4582,24 @@
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
     </row>
-    <row r="15" spans="1:35" ht="259.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="266.25" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>179</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>335</v>
+        <v>287</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>283</v>
+        <v>499</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>231</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>387</v>
+        <v>339</v>
       </c>
       <c r="G15" s="66" t="s">
         <v>28</v>
@@ -4621,16 +4620,16 @@
         <v>3</v>
       </c>
       <c r="M15" s="20" t="s">
-        <v>498</v>
+        <v>450</v>
       </c>
       <c r="N15" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O15" s="24" t="s">
         <v>66</v>
       </c>
       <c r="P15" s="71" t="s">
-        <v>439</v>
+        <v>391</v>
       </c>
       <c r="Q15" s="24" t="s">
         <v>62</v>
@@ -4670,24 +4669,24 @@
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
     </row>
-    <row r="16" spans="1:35" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="168.75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>180</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>336</v>
+        <v>288</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>284</v>
+        <v>500</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>232</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>388</v>
+        <v>340</v>
       </c>
       <c r="G16" s="66" t="s">
         <v>28</v>
@@ -4708,16 +4707,16 @@
         <v>3</v>
       </c>
       <c r="M16" s="20" t="s">
-        <v>499</v>
+        <v>451</v>
       </c>
       <c r="N16" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O16" s="24" t="s">
         <v>69</v>
       </c>
       <c r="P16" s="71" t="s">
-        <v>440</v>
+        <v>392</v>
       </c>
       <c r="Q16" s="24" t="s">
         <v>31</v>
@@ -4757,24 +4756,24 @@
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
     </row>
-    <row r="17" spans="1:35" ht="216" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="222" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>181</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>337</v>
+        <v>289</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>285</v>
+        <v>501</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>233</v>
       </c>
       <c r="F17" s="69" t="s">
-        <v>389</v>
+        <v>341</v>
       </c>
       <c r="G17" s="66" t="s">
         <v>28</v>
@@ -4795,16 +4794,16 @@
         <v>4</v>
       </c>
       <c r="M17" s="20" t="s">
-        <v>500</v>
+        <v>452</v>
       </c>
       <c r="N17" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O17" s="24" t="s">
         <v>71</v>
       </c>
       <c r="P17" s="71" t="s">
-        <v>441</v>
+        <v>393</v>
       </c>
       <c r="Q17" s="24" t="s">
         <v>31</v>
@@ -4844,24 +4843,24 @@
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
     </row>
-    <row r="18" spans="1:35" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="168.75" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>182</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>338</v>
+        <v>290</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>286</v>
+        <v>502</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>234</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>390</v>
+        <v>342</v>
       </c>
       <c r="G18" s="65" t="s">
         <v>28</v>
@@ -4882,16 +4881,16 @@
         <v>4</v>
       </c>
       <c r="M18" s="20" t="s">
-        <v>501</v>
+        <v>453</v>
       </c>
       <c r="N18" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O18" s="19" t="s">
         <v>74</v>
       </c>
       <c r="P18" s="71" t="s">
-        <v>442</v>
+        <v>394</v>
       </c>
       <c r="Q18" s="24" t="s">
         <v>31</v>
@@ -4931,24 +4930,24 @@
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
     </row>
-    <row r="19" spans="1:35" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="165" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>183</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>339</v>
+        <v>291</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>287</v>
+        <v>503</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>235</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>391</v>
+        <v>343</v>
       </c>
       <c r="G19" s="65" t="s">
         <v>28</v>
@@ -4965,16 +4964,16 @@
       <c r="K19" s="38"/>
       <c r="L19" s="38"/>
       <c r="M19" s="20" t="s">
-        <v>502</v>
+        <v>454</v>
       </c>
       <c r="N19" s="28" t="s">
-        <v>477</v>
+        <v>429</v>
       </c>
       <c r="O19" s="19" t="s">
         <v>75</v>
       </c>
       <c r="P19" s="71" t="s">
-        <v>443</v>
+        <v>395</v>
       </c>
       <c r="Q19" s="24" t="s">
         <v>31</v>
@@ -5010,24 +5009,24 @@
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
     </row>
-    <row r="20" spans="1:35" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>184</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>340</v>
+        <v>292</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>288</v>
+        <v>504</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>236</v>
       </c>
       <c r="F20" s="69" t="s">
-        <v>392</v>
+        <v>344</v>
       </c>
       <c r="G20" s="65" t="s">
         <v>28</v>
@@ -5044,16 +5043,16 @@
       <c r="K20" s="38"/>
       <c r="L20" s="38"/>
       <c r="M20" s="20" t="s">
-        <v>503</v>
+        <v>455</v>
       </c>
       <c r="N20" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>76</v>
       </c>
       <c r="P20" s="71" t="s">
-        <v>444</v>
+        <v>396</v>
       </c>
       <c r="Q20" s="24" t="s">
         <v>31</v>
@@ -5089,24 +5088,24 @@
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
     </row>
-    <row r="21" spans="1:35" ht="219" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="219" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>185</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>341</v>
+        <v>293</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>289</v>
+        <v>505</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>237</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>393</v>
+        <v>345</v>
       </c>
       <c r="G21" s="65" t="s">
         <v>28</v>
@@ -5127,16 +5126,16 @@
         <v>4</v>
       </c>
       <c r="M21" s="20" t="s">
-        <v>504</v>
+        <v>456</v>
       </c>
       <c r="N21" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O21" s="72" t="s">
         <v>74</v>
       </c>
       <c r="P21" s="71" t="s">
-        <v>445</v>
+        <v>397</v>
       </c>
       <c r="Q21" s="24" t="s">
         <v>31</v>
@@ -5176,24 +5175,24 @@
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
     </row>
-    <row r="22" spans="1:35" ht="219" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="219" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>186</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>342</v>
+        <v>294</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>290</v>
+        <v>506</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>238</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>394</v>
+        <v>346</v>
       </c>
       <c r="G22" s="65" t="s">
         <v>28</v>
@@ -5214,16 +5213,16 @@
         <v>3</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>505</v>
+        <v>457</v>
       </c>
       <c r="N22" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O22" s="72" t="s">
         <v>77</v>
       </c>
       <c r="P22" s="71" t="s">
-        <v>446</v>
+        <v>398</v>
       </c>
       <c r="Q22" s="24" t="s">
         <v>31</v>
@@ -5263,24 +5262,24 @@
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
     </row>
-    <row r="23" spans="1:35" ht="212.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="212.25" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>187</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>343</v>
+        <v>295</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>291</v>
+        <v>507</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>239</v>
       </c>
       <c r="F23" s="69" t="s">
-        <v>395</v>
+        <v>347</v>
       </c>
       <c r="G23" s="65" t="s">
         <v>28</v>
@@ -5301,16 +5300,16 @@
         <v>4</v>
       </c>
       <c r="M23" s="20" t="s">
-        <v>506</v>
+        <v>458</v>
       </c>
       <c r="N23" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O23" s="19" t="s">
         <v>78</v>
       </c>
       <c r="P23" s="71" t="s">
-        <v>447</v>
+        <v>399</v>
       </c>
       <c r="Q23" s="24" t="s">
         <v>31</v>
@@ -5350,24 +5349,24 @@
       <c r="AH23" s="1"/>
       <c r="AI23" s="1"/>
     </row>
-    <row r="24" spans="1:35" ht="108" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="108" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>188</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>344</v>
+        <v>296</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>292</v>
+        <v>508</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>240</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>396</v>
+        <v>348</v>
       </c>
       <c r="G24" s="65" t="s">
         <v>28</v>
@@ -5388,16 +5387,16 @@
         <v>4</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>507</v>
+        <v>459</v>
       </c>
       <c r="N24" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O24" s="19" t="s">
         <v>79</v>
       </c>
       <c r="P24" s="71" t="s">
-        <v>448</v>
+        <v>400</v>
       </c>
       <c r="Q24" s="24" t="s">
         <v>31</v>
@@ -5437,24 +5436,24 @@
       <c r="AH24" s="1"/>
       <c r="AI24" s="1"/>
     </row>
-    <row r="25" spans="1:35" ht="223.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="223.5" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>189</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>345</v>
+        <v>297</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>293</v>
+        <v>509</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>241</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>397</v>
+        <v>349</v>
       </c>
       <c r="G25" s="65" t="s">
         <v>28</v>
@@ -5475,16 +5474,16 @@
         <v>4</v>
       </c>
       <c r="M25" s="20" t="s">
-        <v>508</v>
+        <v>460</v>
       </c>
       <c r="N25" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O25" s="19" t="s">
         <v>74</v>
       </c>
       <c r="P25" s="71" t="s">
-        <v>449</v>
+        <v>401</v>
       </c>
       <c r="Q25" s="24" t="s">
         <v>31</v>
@@ -5524,24 +5523,24 @@
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
     </row>
-    <row r="26" spans="1:35" ht="174" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="174" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>190</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>346</v>
+        <v>298</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>294</v>
+        <v>510</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>242</v>
       </c>
       <c r="F26" s="69" t="s">
-        <v>398</v>
+        <v>350</v>
       </c>
       <c r="G26" s="65" t="s">
         <v>28</v>
@@ -5562,16 +5561,16 @@
         <v>3</v>
       </c>
       <c r="M26" s="20" t="s">
-        <v>509</v>
+        <v>461</v>
       </c>
       <c r="N26" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O26" s="19" t="s">
         <v>80</v>
       </c>
       <c r="P26" s="71" t="s">
-        <v>450</v>
+        <v>402</v>
       </c>
       <c r="Q26" s="24" t="s">
         <v>31</v>
@@ -5611,24 +5610,24 @@
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
     </row>
-    <row r="27" spans="1:35" ht="127.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>191</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>347</v>
+        <v>299</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>295</v>
+        <v>511</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>243</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>399</v>
+        <v>351</v>
       </c>
       <c r="G27" s="65" t="s">
         <v>28</v>
@@ -5649,16 +5648,16 @@
         <v>4</v>
       </c>
       <c r="M27" s="20" t="s">
-        <v>510</v>
+        <v>462</v>
       </c>
       <c r="N27" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O27" s="19" t="s">
         <v>81</v>
       </c>
       <c r="P27" s="71" t="s">
-        <v>451</v>
+        <v>403</v>
       </c>
       <c r="Q27" s="24" t="s">
         <v>31</v>
@@ -5698,24 +5697,24 @@
       <c r="AH27" s="1"/>
       <c r="AI27" s="1"/>
     </row>
-    <row r="28" spans="1:35" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" ht="180" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>192</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>348</v>
+        <v>300</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>296</v>
+        <v>512</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>244</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>400</v>
+        <v>352</v>
       </c>
       <c r="G28" s="65" t="s">
         <v>28</v>
@@ -5736,16 +5735,16 @@
         <v>3</v>
       </c>
       <c r="M28" s="20" t="s">
-        <v>511</v>
+        <v>463</v>
       </c>
       <c r="N28" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O28" s="19" t="s">
         <v>82</v>
       </c>
       <c r="P28" s="71" t="s">
-        <v>452</v>
+        <v>404</v>
       </c>
       <c r="Q28" s="24" t="s">
         <v>31</v>
@@ -5785,24 +5784,24 @@
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
     </row>
-    <row r="29" spans="1:35" ht="132.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" ht="132.75" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>193</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>349</v>
+        <v>301</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>297</v>
+        <v>513</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>245</v>
       </c>
       <c r="F29" s="69" t="s">
-        <v>401</v>
+        <v>353</v>
       </c>
       <c r="G29" s="65" t="s">
         <v>28</v>
@@ -5823,16 +5822,16 @@
         <v>4</v>
       </c>
       <c r="M29" s="20" t="s">
-        <v>512</v>
+        <v>464</v>
       </c>
       <c r="N29" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O29" s="19" t="s">
         <v>81</v>
       </c>
       <c r="P29" s="71" t="s">
-        <v>452</v>
+        <v>404</v>
       </c>
       <c r="Q29" s="24" t="s">
         <v>31</v>
@@ -5872,24 +5871,24 @@
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
     </row>
-    <row r="30" spans="1:35" ht="223.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="223.5" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>194</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>350</v>
+        <v>302</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>298</v>
+        <v>514</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>246</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>402</v>
+        <v>354</v>
       </c>
       <c r="G30" s="65" t="s">
         <v>28</v>
@@ -5910,16 +5909,16 @@
         <v>4</v>
       </c>
       <c r="M30" s="20" t="s">
-        <v>513</v>
+        <v>465</v>
       </c>
       <c r="N30" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O30" s="19" t="s">
         <v>84</v>
       </c>
       <c r="P30" s="71" t="s">
-        <v>453</v>
+        <v>405</v>
       </c>
       <c r="Q30" s="24" t="s">
         <v>31</v>
@@ -5959,24 +5958,24 @@
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
     </row>
-    <row r="31" spans="1:35" ht="223.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" ht="223.5" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>195</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>351</v>
+        <v>303</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>299</v>
+        <v>515</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>247</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>403</v>
+        <v>355</v>
       </c>
       <c r="G31" s="65" t="s">
         <v>28</v>
@@ -5997,16 +5996,16 @@
         <v>4</v>
       </c>
       <c r="M31" s="20" t="s">
-        <v>514</v>
+        <v>466</v>
       </c>
       <c r="N31" s="28" t="s">
-        <v>478</v>
+        <v>430</v>
       </c>
       <c r="O31" s="19" t="s">
         <v>85</v>
       </c>
       <c r="P31" s="71" t="s">
-        <v>454</v>
+        <v>406</v>
       </c>
       <c r="Q31" s="24" t="s">
         <v>31</v>
@@ -6046,24 +6045,24 @@
       <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
     </row>
-    <row r="32" spans="1:35" ht="133.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="133.5" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>196</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>300</v>
+        <v>516</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>248</v>
       </c>
       <c r="F32" s="69" t="s">
-        <v>404</v>
+        <v>356</v>
       </c>
       <c r="G32" s="65" t="s">
         <v>28</v>
@@ -6084,16 +6083,16 @@
         <v>4</v>
       </c>
       <c r="M32" s="20" t="s">
-        <v>515</v>
+        <v>467</v>
       </c>
       <c r="N32" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="O32" s="19" t="s">
         <v>86</v>
       </c>
       <c r="P32" s="71" t="s">
-        <v>455</v>
+        <v>407</v>
       </c>
       <c r="Q32" s="24" t="s">
         <v>31</v>
@@ -6133,24 +6132,24 @@
       <c r="AH32" s="1"/>
       <c r="AI32" s="1"/>
     </row>
-    <row r="33" spans="1:35" ht="133.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" ht="133.5" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>197</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>301</v>
+        <v>517</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>249</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>405</v>
+        <v>357</v>
       </c>
       <c r="G33" s="65" t="s">
         <v>28</v>
@@ -6171,16 +6170,16 @@
         <v>4</v>
       </c>
       <c r="M33" s="20" t="s">
-        <v>516</v>
+        <v>468</v>
       </c>
       <c r="N33" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="O33" s="19" t="s">
         <v>87</v>
       </c>
       <c r="P33" s="71" t="s">
-        <v>456</v>
+        <v>408</v>
       </c>
       <c r="Q33" s="24" t="s">
         <v>31</v>
@@ -6220,24 +6219,24 @@
       <c r="AH33" s="1"/>
       <c r="AI33" s="1"/>
     </row>
-    <row r="34" spans="1:35" ht="133.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" ht="133.5" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>198</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>302</v>
+        <v>518</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>250</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>406</v>
+        <v>358</v>
       </c>
       <c r="G34" s="65" t="s">
         <v>28</v>
@@ -6258,16 +6257,16 @@
         <v>4</v>
       </c>
       <c r="M34" s="20" t="s">
-        <v>517</v>
+        <v>469</v>
       </c>
       <c r="N34" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="O34" s="19" t="s">
         <v>88</v>
       </c>
       <c r="P34" s="71" t="s">
-        <v>457</v>
+        <v>409</v>
       </c>
       <c r="Q34" s="24" t="s">
         <v>31</v>
@@ -6307,24 +6306,24 @@
       <c r="AH34" s="1"/>
       <c r="AI34" s="1"/>
     </row>
-    <row r="35" spans="1:35" ht="235.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" ht="235.5" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>199</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>355</v>
+        <v>307</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>303</v>
+        <v>519</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>251</v>
       </c>
       <c r="F35" s="69" t="s">
-        <v>407</v>
+        <v>359</v>
       </c>
       <c r="G35" s="65" t="s">
         <v>28</v>
@@ -6345,16 +6344,16 @@
         <v>4</v>
       </c>
       <c r="M35" s="20" t="s">
-        <v>518</v>
+        <v>470</v>
       </c>
       <c r="N35" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="O35" s="19" t="s">
         <v>89</v>
       </c>
       <c r="P35" s="71" t="s">
-        <v>458</v>
+        <v>410</v>
       </c>
       <c r="Q35" s="24" t="s">
         <v>31</v>
@@ -6394,24 +6393,24 @@
       <c r="AH35" s="1"/>
       <c r="AI35" s="1"/>
     </row>
-    <row r="36" spans="1:35" ht="133.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" ht="133.5" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>200</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>356</v>
+        <v>308</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>304</v>
+        <v>520</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>252</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>408</v>
+        <v>360</v>
       </c>
       <c r="G36" s="65" t="s">
         <v>28</v>
@@ -6428,16 +6427,16 @@
       <c r="K36" s="48"/>
       <c r="L36" s="48"/>
       <c r="M36" s="20" t="s">
-        <v>519</v>
+        <v>471</v>
       </c>
       <c r="N36" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="O36" s="19" t="s">
         <v>75</v>
       </c>
       <c r="P36" s="71" t="s">
-        <v>459</v>
+        <v>411</v>
       </c>
       <c r="Q36" s="24" t="s">
         <v>31</v>
@@ -6477,24 +6476,24 @@
       <c r="AH36" s="1"/>
       <c r="AI36" s="1"/>
     </row>
-    <row r="37" spans="1:35" ht="133.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" ht="133.5" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>357</v>
+        <v>309</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>305</v>
+        <v>521</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>253</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>409</v>
+        <v>361</v>
       </c>
       <c r="G37" s="65" t="s">
         <v>57</v>
@@ -6515,16 +6514,16 @@
         <v>4</v>
       </c>
       <c r="M37" s="20" t="s">
-        <v>520</v>
+        <v>472</v>
       </c>
       <c r="N37" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="O37" s="19" t="s">
         <v>90</v>
       </c>
       <c r="P37" s="71" t="s">
-        <v>429</v>
+        <v>381</v>
       </c>
       <c r="Q37" s="24" t="s">
         <v>31</v>
@@ -6564,24 +6563,24 @@
       <c r="AH37" s="1"/>
       <c r="AI37" s="1"/>
     </row>
-    <row r="38" spans="1:35" ht="133.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="133.5" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>202</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>358</v>
+        <v>310</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>306</v>
+        <v>522</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>254</v>
       </c>
       <c r="F38" s="69" t="s">
-        <v>410</v>
+        <v>362</v>
       </c>
       <c r="G38" s="65" t="s">
         <v>57</v>
@@ -6598,16 +6597,16 @@
       <c r="K38" s="48"/>
       <c r="L38" s="48"/>
       <c r="M38" s="20" t="s">
-        <v>521</v>
+        <v>473</v>
       </c>
       <c r="N38" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="O38" s="72" t="s">
         <v>75</v>
       </c>
       <c r="P38" s="71" t="s">
-        <v>461</v>
+        <v>413</v>
       </c>
       <c r="Q38" s="24" t="s">
         <v>31</v>
@@ -6647,30 +6646,30 @@
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
     </row>
-    <row r="39" spans="1:35" ht="174" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="169.5" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>203</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>359</v>
+        <v>311</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>307</v>
+        <v>523</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>255</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>411</v>
+        <v>363</v>
       </c>
       <c r="G39" s="66" t="s">
         <v>28</v>
       </c>
       <c r="H39" s="67" t="s">
-        <v>537</v>
+        <v>489</v>
       </c>
       <c r="I39" s="67" t="s">
         <v>72</v>
@@ -6685,16 +6684,16 @@
         <v>3</v>
       </c>
       <c r="M39" s="20" t="s">
-        <v>522</v>
+        <v>474</v>
       </c>
       <c r="N39" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="O39" s="52" t="s">
         <v>93</v>
       </c>
       <c r="P39" s="71" t="s">
-        <v>460</v>
+        <v>412</v>
       </c>
       <c r="Q39" s="52" t="s">
         <v>31</v>
@@ -6734,30 +6733,30 @@
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
     </row>
-    <row r="40" spans="1:35" ht="174" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="169.5" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>204</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>360</v>
+        <v>312</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>308</v>
+        <v>524</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>256</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>412</v>
+        <v>364</v>
       </c>
       <c r="G40" s="66" t="s">
         <v>28</v>
       </c>
       <c r="H40" s="67" t="s">
-        <v>537</v>
+        <v>489</v>
       </c>
       <c r="I40" s="67" t="s">
         <v>83</v>
@@ -6768,16 +6767,16 @@
       <c r="K40" s="60"/>
       <c r="L40" s="60"/>
       <c r="M40" s="20" t="s">
-        <v>523</v>
+        <v>475</v>
       </c>
       <c r="N40" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="O40" s="21" t="s">
         <v>94</v>
       </c>
       <c r="P40" s="71" t="s">
-        <v>462</v>
+        <v>414</v>
       </c>
       <c r="Q40" s="52" t="s">
         <v>31</v>
@@ -6813,24 +6812,24 @@
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
     </row>
-    <row r="41" spans="1:35" ht="84" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" ht="84" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>205</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>361</v>
+        <v>313</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>309</v>
+        <v>525</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>257</v>
       </c>
       <c r="F41" s="69" t="s">
-        <v>413</v>
+        <v>365</v>
       </c>
       <c r="G41" s="66" t="s">
         <v>28</v>
@@ -6851,16 +6850,16 @@
         <v>4</v>
       </c>
       <c r="M41" s="20" t="s">
-        <v>524</v>
+        <v>476</v>
       </c>
       <c r="N41" s="28" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="O41" s="19" t="s">
         <v>95</v>
       </c>
       <c r="P41" s="71" t="s">
-        <v>463</v>
+        <v>415</v>
       </c>
       <c r="Q41" s="52" t="s">
         <v>31</v>
@@ -6890,13 +6889,13 @@
         <v>48</v>
       </c>
       <c r="Z41" s="19" t="s">
-        <v>483</v>
+        <v>435</v>
       </c>
       <c r="AA41" s="19" t="s">
-        <v>484</v>
+        <v>436</v>
       </c>
       <c r="AB41" s="49" t="s">
-        <v>479</v>
+        <v>431</v>
       </c>
       <c r="AC41" s="58">
         <v>44256</v>
@@ -6908,24 +6907,24 @@
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
     </row>
-    <row r="42" spans="1:35" ht="144.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" ht="145.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="73" t="s">
         <v>206</v>
       </c>
       <c r="B42" s="74" t="s">
-        <v>362</v>
-      </c>
-      <c r="C42" s="75" t="s">
-        <v>310</v>
+        <v>314</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>526</v>
       </c>
       <c r="D42" s="151" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E42" s="73" t="s">
         <v>258</v>
       </c>
       <c r="F42" s="77" t="s">
-        <v>414</v>
+        <v>366</v>
       </c>
       <c r="G42" s="99" t="s">
         <v>28</v>
@@ -6946,16 +6945,16 @@
         <v>4</v>
       </c>
       <c r="M42" s="75" t="s">
-        <v>525</v>
+        <v>477</v>
       </c>
       <c r="N42" s="151" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O42" s="74" t="s">
         <v>96</v>
       </c>
       <c r="P42" s="80" t="s">
-        <v>464</v>
+        <v>416</v>
       </c>
       <c r="Q42" s="101" t="s">
         <v>31</v>
@@ -6985,13 +6984,13 @@
         <v>48</v>
       </c>
       <c r="Z42" s="74" t="s">
-        <v>481</v>
+        <v>433</v>
       </c>
       <c r="AA42" s="74" t="s">
-        <v>482</v>
+        <v>434</v>
       </c>
       <c r="AB42" s="76" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="AC42" s="104">
         <v>44256</v>
@@ -7003,24 +7002,24 @@
       <c r="AH42" s="1"/>
       <c r="AI42" s="1"/>
     </row>
-    <row r="43" spans="1:35" ht="151.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" ht="151.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A43" s="121" t="s">
         <v>207</v>
       </c>
       <c r="B43" s="122" t="s">
-        <v>363</v>
-      </c>
-      <c r="C43" s="123" t="s">
-        <v>311</v>
+        <v>315</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>527</v>
       </c>
       <c r="D43" s="152" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E43" s="124" t="s">
         <v>259</v>
       </c>
       <c r="F43" s="125" t="s">
-        <v>415</v>
+        <v>367</v>
       </c>
       <c r="G43" s="126" t="s">
         <v>57</v>
@@ -7039,16 +7038,16 @@
         <v>4</v>
       </c>
       <c r="M43" s="123" t="s">
-        <v>526</v>
+        <v>478</v>
       </c>
       <c r="N43" s="152" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O43" s="129" t="s">
         <v>99</v>
       </c>
       <c r="P43" s="130" t="s">
-        <v>465</v>
+        <v>417</v>
       </c>
       <c r="Q43" s="129" t="s">
         <v>62</v>
@@ -7088,24 +7087,24 @@
       <c r="AH43" s="1"/>
       <c r="AI43" s="1"/>
     </row>
-    <row r="44" spans="1:35" ht="150.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" ht="150.75" x14ac:dyDescent="0.25">
       <c r="A44" s="135" t="s">
         <v>208</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>364</v>
+        <v>316</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>312</v>
+        <v>528</v>
       </c>
       <c r="D44" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E44" s="18" t="s">
         <v>260</v>
       </c>
       <c r="F44" s="69" t="s">
-        <v>416</v>
+        <v>368</v>
       </c>
       <c r="G44" s="67" t="s">
         <v>57</v>
@@ -7124,16 +7123,16 @@
         <v>3</v>
       </c>
       <c r="M44" s="20" t="s">
-        <v>527</v>
+        <v>479</v>
       </c>
       <c r="N44" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O44" s="30" t="s">
         <v>100</v>
       </c>
       <c r="P44" s="71" t="s">
-        <v>466</v>
+        <v>418</v>
       </c>
       <c r="Q44" s="30" t="s">
         <v>62</v>
@@ -7173,24 +7172,24 @@
       <c r="AH44" s="1"/>
       <c r="AI44" s="1"/>
     </row>
-    <row r="45" spans="1:35" ht="82.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A45" s="135" t="s">
         <v>209</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>365</v>
+        <v>317</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>313</v>
+        <v>529</v>
       </c>
       <c r="D45" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E45" s="18" t="s">
         <v>261</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>417</v>
+        <v>369</v>
       </c>
       <c r="G45" s="67" t="s">
         <v>57</v>
@@ -7209,16 +7208,16 @@
         <v>5</v>
       </c>
       <c r="M45" s="20" t="s">
-        <v>528</v>
+        <v>480</v>
       </c>
       <c r="N45" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O45" s="30" t="s">
         <v>101</v>
       </c>
       <c r="P45" s="71" t="s">
-        <v>467</v>
+        <v>419</v>
       </c>
       <c r="Q45" s="30" t="s">
         <v>31</v>
@@ -7258,24 +7257,24 @@
       <c r="AH45" s="1"/>
       <c r="AI45" s="1"/>
     </row>
-    <row r="46" spans="1:35" ht="143.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" ht="143.25" x14ac:dyDescent="0.25">
       <c r="A46" s="135" t="s">
         <v>210</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>366</v>
+        <v>318</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>314</v>
+        <v>530</v>
       </c>
       <c r="D46" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E46" s="18" t="s">
         <v>262</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>418</v>
+        <v>370</v>
       </c>
       <c r="G46" s="67" t="s">
         <v>57</v>
@@ -7294,16 +7293,16 @@
         <v>2</v>
       </c>
       <c r="M46" s="20" t="s">
-        <v>529</v>
+        <v>481</v>
       </c>
       <c r="N46" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O46" s="30" t="s">
         <v>102</v>
       </c>
       <c r="P46" s="71" t="s">
-        <v>468</v>
+        <v>420</v>
       </c>
       <c r="Q46" s="30" t="s">
         <v>62</v>
@@ -7343,24 +7342,24 @@
       <c r="AH46" s="1"/>
       <c r="AI46" s="1"/>
     </row>
-    <row r="47" spans="1:35" ht="143.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" ht="143.25" x14ac:dyDescent="0.25">
       <c r="A47" s="135" t="s">
         <v>211</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>367</v>
+        <v>319</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>315</v>
+        <v>531</v>
       </c>
       <c r="D47" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E47" s="18" t="s">
         <v>263</v>
       </c>
       <c r="F47" s="69" t="s">
-        <v>419</v>
+        <v>371</v>
       </c>
       <c r="G47" s="67" t="s">
         <v>57</v>
@@ -7379,16 +7378,16 @@
         <v>1</v>
       </c>
       <c r="M47" s="20" t="s">
-        <v>530</v>
+        <v>482</v>
       </c>
       <c r="N47" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O47" s="30" t="s">
         <v>103</v>
       </c>
       <c r="P47" s="71" t="s">
-        <v>469</v>
+        <v>421</v>
       </c>
       <c r="Q47" s="30" t="s">
         <v>62</v>
@@ -7428,24 +7427,24 @@
       <c r="AH47" s="1"/>
       <c r="AI47" s="1"/>
     </row>
-    <row r="48" spans="1:35" ht="78.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:35" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A48" s="135" t="s">
         <v>212</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>368</v>
+        <v>320</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>316</v>
+        <v>532</v>
       </c>
       <c r="D48" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E48" s="18" t="s">
         <v>264</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>420</v>
+        <v>372</v>
       </c>
       <c r="G48" s="67" t="s">
         <v>57</v>
@@ -7464,16 +7463,16 @@
         <v>4</v>
       </c>
       <c r="M48" s="20" t="s">
-        <v>531</v>
+        <v>483</v>
       </c>
       <c r="N48" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O48" s="30" t="s">
         <v>104</v>
       </c>
       <c r="P48" s="71" t="s">
-        <v>470</v>
+        <v>422</v>
       </c>
       <c r="Q48" s="30" t="s">
         <v>62</v>
@@ -7513,24 +7512,24 @@
       <c r="AH48" s="1"/>
       <c r="AI48" s="1"/>
     </row>
-    <row r="49" spans="1:35" ht="79.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="137" t="s">
         <v>213</v>
       </c>
       <c r="B49" s="138" t="s">
-        <v>369</v>
-      </c>
-      <c r="C49" s="139" t="s">
-        <v>317</v>
+        <v>321</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>533</v>
       </c>
       <c r="D49" s="154" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E49" s="140" t="s">
         <v>265</v>
       </c>
       <c r="F49" s="141" t="s">
-        <v>421</v>
+        <v>373</v>
       </c>
       <c r="G49" s="142" t="s">
         <v>57</v>
@@ -7549,16 +7548,16 @@
         <v>2</v>
       </c>
       <c r="M49" s="139" t="s">
-        <v>532</v>
+        <v>484</v>
       </c>
       <c r="N49" s="154" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O49" s="145" t="s">
         <v>106</v>
       </c>
       <c r="P49" s="146" t="s">
-        <v>471</v>
+        <v>423</v>
       </c>
       <c r="Q49" s="145" t="s">
         <v>62</v>
@@ -7598,24 +7597,24 @@
       <c r="AH49" s="1"/>
       <c r="AI49" s="1"/>
     </row>
-    <row r="50" spans="1:35" ht="141" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" ht="141.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A50" s="106" t="s">
         <v>214</v>
       </c>
       <c r="B50" s="107" t="s">
-        <v>370</v>
-      </c>
-      <c r="C50" s="108" t="s">
-        <v>318</v>
+        <v>322</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>534</v>
       </c>
       <c r="D50" s="155" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E50" s="109" t="s">
         <v>266</v>
       </c>
       <c r="F50" s="110" t="s">
-        <v>422</v>
+        <v>374</v>
       </c>
       <c r="G50" s="111" t="s">
         <v>127</v>
@@ -7634,16 +7633,16 @@
         <v>5</v>
       </c>
       <c r="M50" s="108" t="s">
-        <v>533</v>
+        <v>485</v>
       </c>
       <c r="N50" s="155" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O50" s="114" t="s">
         <v>108</v>
       </c>
       <c r="P50" s="115" t="s">
-        <v>472</v>
+        <v>424</v>
       </c>
       <c r="Q50" s="114" t="s">
         <v>31</v>
@@ -7683,24 +7682,24 @@
       <c r="AH50" s="1"/>
       <c r="AI50" s="1"/>
     </row>
-    <row r="51" spans="1:35" ht="141" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" ht="141" x14ac:dyDescent="0.25">
       <c r="A51" s="82" t="s">
         <v>215</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>371</v>
+        <v>323</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>319</v>
+        <v>535</v>
       </c>
       <c r="D51" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E51" s="18" t="s">
         <v>267</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>423</v>
+        <v>375</v>
       </c>
       <c r="G51" s="67" t="s">
         <v>127</v>
@@ -7719,16 +7718,16 @@
         <v>5</v>
       </c>
       <c r="M51" s="20" t="s">
-        <v>534</v>
+        <v>486</v>
       </c>
       <c r="N51" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O51" s="30" t="s">
         <v>109</v>
       </c>
       <c r="P51" s="71" t="s">
-        <v>473</v>
+        <v>425</v>
       </c>
       <c r="Q51" s="30" t="s">
         <v>31</v>
@@ -7768,24 +7767,24 @@
       <c r="AH51" s="1"/>
       <c r="AI51" s="1"/>
     </row>
-    <row r="52" spans="1:35" ht="203.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" ht="203.25" x14ac:dyDescent="0.25">
       <c r="A52" s="82" t="s">
         <v>216</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>372</v>
+        <v>324</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>320</v>
+        <v>536</v>
       </c>
       <c r="D52" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E52" s="18" t="s">
         <v>268</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>424</v>
+        <v>376</v>
       </c>
       <c r="G52" s="67" t="s">
         <v>127</v>
@@ -7804,16 +7803,16 @@
         <v>5</v>
       </c>
       <c r="M52" s="20" t="s">
-        <v>535</v>
+        <v>487</v>
       </c>
       <c r="N52" s="153" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O52" s="30" t="s">
         <v>110</v>
       </c>
       <c r="P52" s="71" t="s">
-        <v>474</v>
+        <v>426</v>
       </c>
       <c r="Q52" s="30" t="s">
         <v>62</v>
@@ -7853,24 +7852,24 @@
       <c r="AH52" s="1"/>
       <c r="AI52" s="1"/>
     </row>
-    <row r="53" spans="1:35" ht="141.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" ht="141.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="84" t="s">
         <v>217</v>
       </c>
       <c r="B53" s="85" t="s">
-        <v>373</v>
-      </c>
-      <c r="C53" s="86" t="s">
-        <v>321</v>
+        <v>325</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>537</v>
       </c>
       <c r="D53" s="156" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="E53" s="87" t="s">
         <v>269</v>
       </c>
       <c r="F53" s="88" t="s">
-        <v>425</v>
+        <v>377</v>
       </c>
       <c r="G53" s="89" t="s">
         <v>127</v>
@@ -7889,16 +7888,16 @@
         <v>1</v>
       </c>
       <c r="M53" s="86" t="s">
-        <v>536</v>
+        <v>488</v>
       </c>
       <c r="N53" s="156" t="s">
-        <v>480</v>
+        <v>432</v>
       </c>
       <c r="O53" s="92" t="s">
         <v>111</v>
       </c>
       <c r="P53" s="93" t="s">
-        <v>475</v>
+        <v>427</v>
       </c>
       <c r="Q53" s="92" t="s">
         <v>31</v>
@@ -7938,7 +7937,7 @@
       <c r="AH53" s="1"/>
       <c r="AI53" s="1"/>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="AE54" s="1"/>
       <c r="AF54" s="1"/>
       <c r="AG54" s="1"/>
@@ -10305,18 +10304,7 @@
       <c r="AI391" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD53" xr:uid="{6EE89437-0902-44FC-8D89-0413032D4EE9}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Operational Risk"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters>
-        <filter val="egulatory &amp; Compliance Risk"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AD53" xr:uid="{6EE89437-0902-44FC-8D89-0413032D4EE9}"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added in action_id column to spreadsheet
</commit_message>
<xml_diff>
--- a/clensed.xlsx
+++ b/clensed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PythonProjects\wip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BE532A-A47D-408C-AF36-621393BAE501}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D68DA97-7ED2-441D-8208-791CC7FCB7B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7757194A-FA31-4D25-A9B8-7AE7E2677B79}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7757194A-FA31-4D25-A9B8-7AE7E2677B79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="542">
   <si>
     <t>Process (Title)</t>
   </si>
@@ -2142,6 +2142,18 @@
   </si>
   <si>
     <t>DP-P01-R33</t>
+  </si>
+  <si>
+    <t>Action ID</t>
+  </si>
+  <si>
+    <t>jane Doe</t>
+  </si>
+  <si>
+    <t>An action</t>
+  </si>
+  <si>
+    <t>A description</t>
   </si>
 </sst>
 </file>
@@ -2537,7 +2549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2998,6 +3010,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3316,7 +3331,7 @@
   <dimension ref="A1:AI391"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3445,7 +3460,9 @@
       <c r="AD1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1"/>
+      <c r="AE1" s="157" t="s">
+        <v>538</v>
+      </c>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
@@ -3614,10 +3631,18 @@
       <c r="Y3" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="20"/>
-      <c r="AC3" s="24"/>
+      <c r="Z3" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="AA3" s="19" t="s">
+        <v>541</v>
+      </c>
+      <c r="AB3" s="20" t="s">
+        <v>539</v>
+      </c>
+      <c r="AC3" s="31">
+        <v>44542</v>
+      </c>
       <c r="AD3" s="27"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
@@ -3799,7 +3824,7 @@
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
     </row>
-    <row r="6" spans="1:35" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" ht="180.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>170</v>
       </c>
@@ -3886,7 +3911,7 @@
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
     </row>
-    <row r="7" spans="1:35" ht="116.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" ht="114" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>171</v>
       </c>
@@ -3973,7 +3998,7 @@
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
     </row>
-    <row r="8" spans="1:35" ht="136.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="132.75" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>172</v>
       </c>
@@ -4060,7 +4085,7 @@
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
     </row>
-    <row r="9" spans="1:35" ht="116.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="114" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>173</v>
       </c>
@@ -4147,7 +4172,7 @@
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
     </row>
-    <row r="10" spans="1:35" ht="149.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="145.5" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>174</v>
       </c>
@@ -4234,7 +4259,7 @@
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
     </row>
-    <row r="11" spans="1:35" ht="160.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="156" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>175</v>
       </c>
@@ -4321,7 +4346,7 @@
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
     </row>
-    <row r="12" spans="1:35" ht="160.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="156" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>176</v>
       </c>
@@ -4408,7 +4433,7 @@
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
     </row>
-    <row r="13" spans="1:35" ht="168.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>177</v>
       </c>
@@ -4495,7 +4520,7 @@
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
     </row>
-    <row r="14" spans="1:35" ht="168.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="165" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>178</v>
       </c>
@@ -4582,7 +4607,7 @@
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
     </row>
-    <row r="15" spans="1:35" ht="266.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="259.5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>179</v>
       </c>
@@ -4669,7 +4694,7 @@
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
     </row>
-    <row r="16" spans="1:35" ht="168.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>180</v>
       </c>
@@ -4756,7 +4781,7 @@
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
     </row>
-    <row r="17" spans="1:35" ht="222" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="216" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>181</v>
       </c>
@@ -4843,7 +4868,7 @@
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
     </row>
-    <row r="18" spans="1:35" ht="168.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>182</v>
       </c>

</xml_diff>